<commit_message>
https://github.com/kohei-okazaki/work-3g/issues/1035  - 問い合わせ通知をTOP画面に追加  - その他軽微な修正
</commit_message>
<xml_diff>
--- a/ha-asset/01_design/00_機能一覧.xlsx
+++ b/ha-asset/01_design/00_機能一覧.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\git\work-3g\ha-asset\01_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B786EE-F352-4E8A-B0DF-D579DC93C53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD969EB-3E23-429D-B3C6-CC93F60E27F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11550" yWindow="1110" windowWidth="17160" windowHeight="14295" tabRatio="785" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00_更新履歴" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="249">
   <si>
     <t>更新日</t>
   </si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>バッチファイル名</t>
-  </si>
-  <si>
-    <t>Batchクラス名</t>
   </si>
   <si>
     <t>healthInfoFileRegist.bat</t>
@@ -1061,22 +1058,6 @@
     <phoneticPr fontId="8"/>
   </si>
   <si>
-    <t>jp.co.ha.batch.healthInfoMigrateBatch.HealthInfoMigrateBatch</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>jp.co.ha.batch.healthInfoFileRegist.HealthInfoFileRegistBatch</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>jp.co.ha.batch.healthcheck.HealthCheckApiBatch</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>jp.co.ha.batch.monthlyHealthInfoSummary.MonthlyHealthInfoSummaryBatch</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
     <t>実装に合わせ最新化</t>
     <rPh sb="0" eb="2">
       <t>ジッソウ</t>
@@ -1246,6 +1227,50 @@
   </si>
   <si>
     <t>jp.co.ha.root.contents.inquiry.controller.InquiryNoticeApiController</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>AWS SQS取込バッチ</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>データパージバッチ</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>dataPurge.bat</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>awsQueueImport.bat</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>Configクラス名</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.healthcheck.HealthCheckConfig</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.healthInfoFileRegist.HealthInfoFileRegistConfig</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.datapurge.DataPurgeConfig</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.healthInfoMigrate.HealthInfoMigrateConfig</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.monthlyHealthInfoSummary.MonthlyHealthInfoSummaryConfig</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>jp.co.ha.batch.sqsImport.AwsSqsImportConfig</t>
     <phoneticPr fontId="8"/>
   </si>
 </sst>
@@ -2349,9 +2374,9 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="18.75"/>
@@ -2377,10 +2402,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="56" t="s">
         <v>109</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>110</v>
       </c>
       <c r="E3" s="52"/>
     </row>
@@ -2476,7 +2501,7 @@
         <v>1.07</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="33">
@@ -2488,7 +2513,7 @@
         <v>1.08</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="49.5">
@@ -2500,7 +2525,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="66">
@@ -2512,7 +2537,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2524,7 +2549,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2536,16 +2561,20 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="str">
+      <c r="B17" s="4">
+        <v>45965</v>
+      </c>
+      <c r="C17" s="5">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D17" s="3"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="4"/>
@@ -2751,7 +2780,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="20"/>
@@ -2787,7 +2816,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>31</v>
@@ -2800,10 +2829,10 @@
     <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="11"/>
       <c r="B12" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="20"/>
@@ -2812,10 +2841,10 @@
     <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="11"/>
       <c r="B13" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="20"/>
@@ -2827,7 +2856,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -2839,7 +2868,7 @@
         <v>34</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="19"/>
@@ -3102,26 +3131,26 @@
     <row r="35" spans="1:6" ht="19.5" customHeight="1">
       <c r="A35" s="11"/>
       <c r="B35" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="E35" s="23" t="s">
         <v>226</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>231</v>
       </c>
       <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1">
       <c r="A36" s="11"/>
       <c r="B36" s="17" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="20"/>
@@ -3130,10 +3159,10 @@
     <row r="37" spans="1:6" ht="19.5" customHeight="1">
       <c r="A37" s="11"/>
       <c r="B37" s="17" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="19"/>
@@ -3234,7 +3263,7 @@
     <row r="3" spans="1:7" ht="19.5">
       <c r="A3" s="9"/>
       <c r="B3" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>85</v>
@@ -3259,10 +3288,10 @@
         <v>87</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>88</v>
@@ -3471,9 +3500,9 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="18.75"/>
@@ -3508,13 +3537,13 @@
     <row r="3" spans="1:6" ht="19.5">
       <c r="A3" s="9"/>
       <c r="B3" s="47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="47" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>98</v>
+        <v>242</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>12</v>
@@ -3524,78 +3553,90 @@
     <row r="4" spans="1:6">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>120</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="11"/>
       <c r="B5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="40" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>102</v>
       </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11"/>
       <c r="B6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>104</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>105</v>
       </c>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="11"/>
       <c r="B7" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="11"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="24"/>
+      <c r="B8" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>248</v>
+      </c>
       <c r="E8" s="40"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="11"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="35"/>
+      <c r="B9" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>245</v>
+      </c>
       <c r="E9" s="40"/>
       <c r="F9" s="15"/>
     </row>
@@ -3759,7 +3800,7 @@
     <row r="3" spans="1:9" ht="19.5">
       <c r="A3" s="9"/>
       <c r="B3" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>85</v>
@@ -3778,101 +3819,101 @@
     <row r="4" spans="1:9">
       <c r="A4" s="11"/>
       <c r="B4" s="62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" s="15"/>
       <c r="I4" s="67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="11"/>
       <c r="B5" s="65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F5" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G5" s="15"/>
       <c r="I5" s="67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="11"/>
       <c r="B6" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="11"/>
       <c r="B7" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="11"/>
       <c r="B8" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" s="15"/>
     </row>
@@ -4066,7 +4107,7 @@
     <row r="3" spans="1:7" ht="19.5">
       <c r="A3" s="9"/>
       <c r="B3" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>85</v>
@@ -4085,47 +4126,47 @@
     <row r="4" spans="1:7">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11"/>
       <c r="B5" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="11"/>
       <c r="B6" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="59"/>
@@ -4134,10 +4175,10 @@
     <row r="7" spans="1:7">
       <c r="A7" s="11"/>
       <c r="B7" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="17"/>
@@ -4147,10 +4188,10 @@
     <row r="8" spans="1:7">
       <c r="A8" s="11"/>
       <c r="B8" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="17"/>
@@ -4160,30 +4201,30 @@
     <row r="9" spans="1:7">
       <c r="A9" s="11"/>
       <c r="B9" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="11"/>
       <c r="B10" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="60"/>
@@ -4192,13 +4233,13 @@
     <row r="11" spans="1:7">
       <c r="A11" s="11"/>
       <c r="B11" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="25"/>
@@ -4207,30 +4248,30 @@
     <row r="12" spans="1:7">
       <c r="A12" s="11"/>
       <c r="B12" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="11"/>
       <c r="B13" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -4239,47 +4280,47 @@
     <row r="14" spans="1:7">
       <c r="A14" s="11"/>
       <c r="B14" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="11"/>
       <c r="B15" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="11"/>
       <c r="B16" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -4288,30 +4329,30 @@
     <row r="17" spans="1:7">
       <c r="A17" s="11"/>
       <c r="B17" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="11"/>
       <c r="B18" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="59"/>
@@ -4320,13 +4361,13 @@
     <row r="19" spans="1:7">
       <c r="A19" s="11"/>
       <c r="B19" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="60"/>
@@ -4335,13 +4376,13 @@
     <row r="20" spans="1:7">
       <c r="A20" s="58"/>
       <c r="B20" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
@@ -4350,30 +4391,30 @@
     <row r="21" spans="1:7">
       <c r="A21" s="58"/>
       <c r="B21" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G21" s="58"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="58"/>
       <c r="B22" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="59"/>
@@ -4382,13 +4423,13 @@
     <row r="23" spans="1:7">
       <c r="A23" s="58"/>
       <c r="B23" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="60"/>
@@ -4397,13 +4438,13 @@
     <row r="24" spans="1:7">
       <c r="A24" s="58"/>
       <c r="B24" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
@@ -4412,47 +4453,47 @@
     <row r="25" spans="1:7">
       <c r="A25" s="58"/>
       <c r="B25" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G25" s="58"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="58"/>
       <c r="B26" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="35" t="s">
         <v>233</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>238</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="68" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G26" s="58"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="58"/>
       <c r="B27" s="17" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="69"/>
@@ -4461,13 +4502,13 @@
     <row r="28" spans="1:7">
       <c r="A28" s="58"/>
       <c r="B28" s="17" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="70"/>

</xml_diff>